<commit_message>
GK: fixed "slop" to "slope" in all of the code
</commit_message>
<xml_diff>
--- a/create_forecast_basic/future/JTMT/Monitoring/240908_pivot_by_muni_forecast_pop_jewish_till_2050_jtmt.xlsx
+++ b/create_forecast_basic/future/JTMT/Monitoring/240908_pivot_by_muni_forecast_pop_jewish_till_2050_jtmt.xlsx
@@ -1394,7 +1394,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">הר חברון_x000D_
+          <t xml:space="preserve">הר חברון
 </t>
         </is>
       </c>
@@ -1623,7 +1623,7 @@
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">מגילות ים המלח_x000D_
+          <t xml:space="preserve">מגילות ים המלח
 </t>
         </is>
       </c>
@@ -2232,7 +2232,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">ערבות הירדן_x000D_
+          <t xml:space="preserve">ערבות הירדן
 </t>
         </is>
       </c>

</xml_diff>